<commit_message>
im ok im ok deep breathing im ok im good im ok
</commit_message>
<xml_diff>
--- a/document/db/DB명세서.xlsx
+++ b/document/db/DB명세서.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="91">
   <si>
     <t xml:space="preserve">Table </t>
   </si>
@@ -97,9 +97,6 @@
     <t>close</t>
   </si>
   <si>
-    <t>MainTopic_TopicTag</t>
-  </si>
-  <si>
     <t>tag_id</t>
   </si>
   <si>
@@ -217,9 +214,6 @@
     <t>반대갯수</t>
   </si>
   <si>
-    <t>대주제 등록된 날짜및 시간</t>
-  </si>
-  <si>
     <t>대주제 닫혔는지 여부</t>
   </si>
   <si>
@@ -235,21 +229,12 @@
     <t>찬성이나 반대의 의견</t>
   </si>
   <si>
-    <t>그림이나 그외 바이너리 파일들</t>
-  </si>
-  <si>
     <t>의견의 명예점수</t>
   </si>
   <si>
-    <t>참여요청했는지 참여중인건지</t>
-  </si>
-  <si>
     <t>신고당한 횟수</t>
   </si>
   <si>
-    <t>찬성 또는 반대 또는 중립</t>
-  </si>
-  <si>
     <t>소주제</t>
   </si>
   <si>
@@ -257,9 +242,6 @@
   </si>
   <si>
     <t>소주제 종료타임</t>
-  </si>
-  <si>
-    <t>소주제 닫혔는지 여부</t>
   </si>
   <si>
     <t>대주제 태그</t>
@@ -285,6 +267,34 @@
   </si>
   <si>
     <t>VARCHAR</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>참여중, 요청 여부</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>MainTopic_TopicTag</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>interest id</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>대주제 등록 날짜,시간</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>그림,바이너리 파일들</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>찬성 반대 중립</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>소주제 닫혔는지 여부</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -292,7 +302,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -453,6 +463,41 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -641,7 +686,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -758,77 +803,17 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="4"/>
+        <color theme="4" tint="0.39997558519241921"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
-        <color theme="4"/>
+        <color theme="4" tint="0.39997558519241921"/>
       </right>
       <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+        <color theme="4" tint="0.39997558519241921"/>
       </top>
       <bottom style="thin">
-        <color theme="4"/>
+        <color theme="4" tint="0.39997558519241921"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="4"/>
-      </right>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="4"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="4"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -960,45 +945,27 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1342,21 +1309,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="G49" sqref="A1:G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5" customWidth="1"/>
-    <col min="6" max="6" width="4.75" customWidth="1"/>
-    <col min="7" max="7" width="29.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1378,12 +1344,12 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>88</v>
+      <c r="G1" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1401,17 +1367,17 @@
       <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>58</v>
+      <c r="G2" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
+      <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>3</v>
@@ -1422,19 +1388,19 @@
       <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>59</v>
+      <c r="G3" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>9</v>
@@ -1445,17 +1411,17 @@
       <c r="F4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>60</v>
+      <c r="G4" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
+      <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>9</v>
@@ -1466,12 +1432,12 @@
       <c r="F5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>60</v>
+      <c r="G5" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1489,17 +1455,17 @@
       <c r="F6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>61</v>
+      <c r="G6" s="4" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
+      <c r="A7" s="3"/>
       <c r="B7" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>3</v>
@@ -1510,12 +1476,12 @@
       <c r="F7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>62</v>
+      <c r="G7" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1533,17 +1499,17 @@
       <c r="F8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>63</v>
+      <c r="G8" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="11"/>
+      <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>9</v>
@@ -1554,12 +1520,12 @@
       <c r="F9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>64</v>
+      <c r="G9" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
+      <c r="A10" s="3"/>
       <c r="B10" s="4" t="s">
         <v>22</v>
       </c>
@@ -1575,12 +1541,12 @@
       <c r="F10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>65</v>
+      <c r="G10" s="4" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
+      <c r="A11" s="3"/>
       <c r="B11" s="4" t="s">
         <v>23</v>
       </c>
@@ -1596,12 +1562,12 @@
       <c r="F11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>66</v>
+      <c r="G11" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
+      <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
         <v>24</v>
       </c>
@@ -1617,17 +1583,17 @@
       <c r="F12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>67</v>
+      <c r="G12" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
+      <c r="A13" s="3"/>
       <c r="B13" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>3</v>
@@ -1638,17 +1604,17 @@
       <c r="F13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>68</v>
+      <c r="G13" s="4" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
+      <c r="A14" s="3"/>
       <c r="B14" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>9</v>
@@ -1659,13 +1625,13 @@
       <c r="F14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="6" t="s">
-        <v>60</v>
+      <c r="G14" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
-        <v>27</v>
+      <c r="A15" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>20</v>
@@ -1682,14 +1648,14 @@
       <c r="F15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>63</v>
+      <c r="G15" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
+      <c r="A16" s="3"/>
       <c r="B16" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>8</v>
@@ -1703,19 +1669,19 @@
       <c r="F16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
-        <v>29</v>
+      <c r="G16" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>9</v>
@@ -1726,38 +1692,38 @@
       <c r="F17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
+      <c r="G17" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>3</v>
@@ -1768,11 +1734,14 @@
       <c r="F19" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="6"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
-        <v>33</v>
+      <c r="G19" s="4"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>20</v>
@@ -1789,14 +1758,17 @@
       <c r="F20" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="11"/>
+      <c r="G20" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>8</v>
@@ -1810,14 +1782,17 @@
       <c r="F21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G21" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
+      <c r="G21" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
       <c r="B22" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>8</v>
@@ -1831,17 +1806,20 @@
       <c r="F22" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="11"/>
+      <c r="G22" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
       <c r="B23" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>3</v>
@@ -1852,17 +1830,20 @@
       <c r="F23" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="11"/>
+      <c r="G23" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>3</v>
@@ -1873,17 +1854,20 @@
       <c r="F24" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G24" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="11"/>
+      <c r="G24" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="3"/>
       <c r="B25" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>9</v>
@@ -1894,14 +1878,17 @@
       <c r="F25" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G25" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="12"/>
+      <c r="G25" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
       <c r="B26" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>8</v>
@@ -1915,13 +1902,16 @@
       <c r="F26" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G26" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
-        <v>40</v>
+      <c r="G26" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>20</v>
@@ -1938,17 +1928,20 @@
       <c r="F27" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G27" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="11"/>
+      <c r="G27" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="3"/>
       <c r="B28" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>9</v>
@@ -1959,35 +1952,41 @@
       <c r="F28" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G28" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="11"/>
+      <c r="G28" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="3"/>
       <c r="B29" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="3"/>
+      <c r="B30" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="11"/>
-      <c r="B30" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>8</v>
@@ -2001,17 +2000,20 @@
       <c r="F30" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G30" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="12"/>
+      <c r="G30" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="3"/>
       <c r="B31" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>3</v>
@@ -2022,16 +2024,19 @@
       <c r="F31" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G31" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="s">
-        <v>44</v>
+      <c r="G31" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>8</v>
@@ -2045,12 +2050,15 @@
       <c r="F32" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G32" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="11"/>
+      <c r="G32" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="3"/>
       <c r="B33" s="4" t="s">
         <v>20</v>
       </c>
@@ -2066,35 +2074,41 @@
       <c r="F33" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G33" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="11"/>
+      <c r="G33" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="3"/>
       <c r="B34" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="3"/>
+      <c r="B35" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="11"/>
-      <c r="B35" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>25</v>
@@ -2108,14 +2122,17 @@
       <c r="F35" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G35" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="11"/>
+      <c r="G35" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="3"/>
       <c r="B36" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>25</v>
@@ -2129,17 +2146,20 @@
       <c r="F36" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G36" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="12"/>
+      <c r="G36" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="3"/>
       <c r="B37" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>3</v>
@@ -2150,16 +2170,19 @@
       <c r="F37" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G37" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="10" t="s">
-        <v>49</v>
+      <c r="G37" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>8</v>
@@ -2173,17 +2196,20 @@
       <c r="F38" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G38" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="12"/>
+      <c r="G38" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="3"/>
       <c r="B39" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>3</v>
@@ -2194,19 +2220,22 @@
       <c r="F39" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G39" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="10" t="s">
-        <v>51</v>
+      <c r="G39" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>9</v>
@@ -2217,38 +2246,44 @@
       <c r="F40" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G40" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="11"/>
+      <c r="G40" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="3"/>
       <c r="B41" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="6"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="3"/>
+      <c r="B42" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="11"/>
-      <c r="B42" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="C42" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>3</v>
@@ -2259,17 +2294,20 @@
       <c r="F42" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G42" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="11"/>
+      <c r="G42" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="6"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="3"/>
       <c r="B43" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>9</v>
@@ -2280,14 +2318,17 @@
       <c r="F43" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G43" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="11"/>
+      <c r="G43" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
+      <c r="K43" s="6"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" s="3"/>
       <c r="B44" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>8</v>
@@ -2301,14 +2342,17 @@
       <c r="F44" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G44" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="12"/>
+      <c r="G44" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I44" s="6"/>
+      <c r="J44" s="6"/>
+      <c r="K44" s="6"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" s="3"/>
       <c r="B45" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>8</v>
@@ -2322,19 +2366,19 @@
       <c r="F45" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G45" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="10" t="s">
-        <v>56</v>
+      <c r="G45" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>9</v>
@@ -2345,12 +2389,12 @@
       <c r="F46" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G46" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="12"/>
+      <c r="G46" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" s="3"/>
       <c r="B47" s="4" t="s">
         <v>7</v>
       </c>
@@ -2366,19 +2410,19 @@
       <c r="F47" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G47" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="10" t="s">
+      <c r="G47" s="4" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>9</v>
@@ -2389,33 +2433,39 @@
       <c r="F48" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G48" s="6" t="s">
-        <v>60</v>
+      <c r="G48" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="12"/>
-      <c r="B49" s="7" t="s">
+      <c r="A49" s="3"/>
+      <c r="B49" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C49" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D49" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F49" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G49" s="9" t="s">
-        <v>61</v>
+      <c r="D49" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="A15:A16"/>
     <mergeCell ref="A48:A49"/>
     <mergeCell ref="A20:A26"/>
     <mergeCell ref="A27:A31"/>
@@ -2423,14 +2473,9 @@
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="A40:A45"/>
     <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A14"/>
-    <mergeCell ref="A15:A16"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>